<commit_message>
add tsvs and plots
</commit_message>
<xml_diff>
--- a/Plots/results.xlsx
+++ b/Plots/results.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6135" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6135" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="J48" sheetId="1" r:id="rId1"/>
     <sheet name="OneRule" sheetId="2" r:id="rId2"/>
+    <sheet name="RandomForest" sheetId="3" r:id="rId3"/>
+    <sheet name="ANNs" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="65">
   <si>
     <t>J48 Decision Tree</t>
   </si>
@@ -154,6 +156,72 @@
   </si>
   <si>
     <t>42.93</t>
+  </si>
+  <si>
+    <t>Forest Size</t>
+  </si>
+  <si>
+    <t>76.00</t>
+  </si>
+  <si>
+    <t>81.85</t>
+  </si>
+  <si>
+    <t>84.48</t>
+  </si>
+  <si>
+    <t>85.91</t>
+  </si>
+  <si>
+    <t>Single Layer ANN</t>
+  </si>
+  <si>
+    <t>Learning Rate</t>
+  </si>
+  <si>
+    <t>Epoches</t>
+  </si>
+  <si>
+    <t>88.52</t>
+  </si>
+  <si>
+    <t>87.44</t>
+  </si>
+  <si>
+    <t>87.85</t>
+  </si>
+  <si>
+    <t>88.38</t>
+  </si>
+  <si>
+    <t>87.12</t>
+  </si>
+  <si>
+    <t>87.49</t>
+  </si>
+  <si>
+    <t>87.30</t>
+  </si>
+  <si>
+    <t>86.34</t>
+  </si>
+  <si>
+    <t>86.14</t>
+  </si>
+  <si>
+    <t>85.35</t>
+  </si>
+  <si>
+    <t>84.01</t>
+  </si>
+  <si>
+    <t>83.22</t>
+  </si>
+  <si>
+    <t>81.59</t>
+  </si>
+  <si>
+    <t>79.34</t>
   </si>
 </sst>
 </file>
@@ -718,7 +786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="A2:B7"/>
     </sheetView>
   </sheetViews>
@@ -778,4 +846,263 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="A1:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>50</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>100</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="A2:C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>